<commit_message>
MH update to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_MH.xlsx
+++ b/curation/draft/collection/collection_specialization_MH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0EF36C-8E27-EB4A-B2EF-CD0D8C379249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C8A63-4769-D241-838E-B64ACF081A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Collection_MH" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_MH!$A$1:$AG$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_MH!$A$1:$AH$25</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="119">
   <si>
     <t>package_date</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>Medical History Prespecified: Alzheimer's Disease (Denormalized)</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,16 +480,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -791,12 +789,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -807,24 +805,24 @@
     <col min="5" max="5" width="8.83203125" style="2"/>
     <col min="8" max="8" width="29.83203125" customWidth="1"/>
     <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
-    <col min="11" max="11" width="30.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="41.5" customWidth="1"/>
-    <col min="16" max="16" width="23" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" customWidth="1"/>
-    <col min="23" max="23" width="18.6640625" customWidth="1"/>
-    <col min="24" max="24" width="24.5" customWidth="1"/>
-    <col min="28" max="28" width="15.33203125" customWidth="1"/>
-    <col min="29" max="29" width="25" customWidth="1"/>
-    <col min="30" max="30" width="29.33203125" customWidth="1"/>
-    <col min="31" max="31" width="23.83203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="30.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.5" customWidth="1"/>
+    <col min="17" max="17" width="23" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" customWidth="1"/>
+    <col min="24" max="24" width="18.6640625" customWidth="1"/>
+    <col min="25" max="25" width="24.5" customWidth="1"/>
+    <col min="29" max="29" width="15.33203125" customWidth="1"/>
+    <col min="30" max="30" width="25" customWidth="1"/>
+    <col min="31" max="31" width="29.33203125" customWidth="1"/>
+    <col min="32" max="32" width="23.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -855,1599 +853,1607 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="6" customFormat="1" ht="16">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:34" ht="16">
+      <c r="B2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="9" t="s">
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="6">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="6">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Y2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Z2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AA2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" t="s">
         <v>61</v>
       </c>
-      <c r="AE2" s="10" t="s">
+      <c r="AF2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="6" customFormat="1" ht="16">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:34" ht="16">
+      <c r="B3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="6">
+      <c r="U3">
         <v>10</v>
       </c>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AD3" s="6" t="s">
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AE3" t="s">
         <v>40</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AF3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:34" ht="32">
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" t="s">
         <v>110</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="Q4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="T4" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="6">
+      <c r="U4">
         <v>200</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="W4" t="s">
         <v>45</v>
       </c>
-      <c r="AB4" s="10" t="s">
+      <c r="AC4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AE4" t="s">
         <v>52</v>
       </c>
-      <c r="AE4" s="10" t="s">
+      <c r="AF4" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:34" ht="32">
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" t="s">
         <v>80</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" t="s">
         <v>81</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="Q5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="6">
+      <c r="U5">
         <v>200</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="W5" t="s">
         <v>45</v>
       </c>
-      <c r="AD5" s="6" t="s">
+      <c r="AE5" t="s">
         <v>80</v>
       </c>
-      <c r="AE5" s="10" t="s">
+      <c r="AF5" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:34" ht="32">
+      <c r="B6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" t="s">
         <v>110</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="N6" t="s">
         <v>69</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="S6" t="s">
         <v>54</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="T6" t="s">
         <v>70</v>
       </c>
-      <c r="T6" s="6">
+      <c r="U6">
         <v>2</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AE6" t="s">
         <v>69</v>
       </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AF6" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:34" ht="32">
+      <c r="B7" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="Q7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" t="s">
         <v>45</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="T7" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="6">
+      <c r="U7">
         <v>200</v>
       </c>
-      <c r="AD7" s="6" t="s">
+      <c r="AE7" t="s">
         <v>43</v>
       </c>
-      <c r="AE7" s="10" t="s">
+      <c r="AF7" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:34" ht="32">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="6" t="s">
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" t="s">
         <v>110</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="M8" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="N8" t="s">
         <v>47</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="Q8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8">
         <v>5</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="S8" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="T8" t="s">
         <v>64</v>
       </c>
-      <c r="T8" s="6">
+      <c r="U8">
         <v>10</v>
       </c>
-      <c r="AD8" s="6" t="s">
+      <c r="AE8" t="s">
         <v>48</v>
       </c>
-      <c r="AE8" s="10" t="s">
+      <c r="AF8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:34" ht="32">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" t="s">
         <v>110</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="L9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10" t="s">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9">
         <v>6</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="S9" t="s">
         <v>54</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="T9" t="s">
         <v>46</v>
       </c>
-      <c r="T9" s="6">
+      <c r="U9">
         <v>1</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="X9" t="s">
         <v>59</v>
       </c>
-      <c r="X9" s="11" t="s">
+      <c r="Y9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y9" s="10" t="s">
+      <c r="Z9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z9" s="10" t="s">
+      <c r="AA9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA9" s="6" t="s">
+      <c r="AB9" t="s">
         <v>61</v>
       </c>
-      <c r="AD9" s="6" t="s">
+      <c r="AE9" t="s">
         <v>74</v>
       </c>
-      <c r="AE9" s="10" t="s">
+      <c r="AF9" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="1:34" ht="32">
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="M10" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="N10" t="s">
         <v>50</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="O10" t="s">
         <v>57</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="Q10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10">
         <v>7</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="S10" t="s">
         <v>54</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="T10" t="s">
         <v>64</v>
       </c>
-      <c r="T10" s="6">
+      <c r="U10">
         <v>10</v>
       </c>
-      <c r="AD10" s="6" t="s">
+      <c r="AE10" t="s">
         <v>51</v>
       </c>
-      <c r="AE10" s="10" t="s">
+      <c r="AF10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="6" customFormat="1" ht="48">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:34" ht="48">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="6" t="s">
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
         <v>109</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="L11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="M11" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="N11" t="s">
         <v>49</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="O11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="Q11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="S11" t="s">
         <v>54</v>
       </c>
-      <c r="S11" s="6" t="s">
+      <c r="T11" t="s">
         <v>46</v>
       </c>
-      <c r="T11" s="6">
+      <c r="U11">
         <v>1</v>
       </c>
-      <c r="W11" s="6" t="s">
+      <c r="X11" t="s">
         <v>59</v>
       </c>
-      <c r="X11" s="11" t="s">
+      <c r="Y11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y11" s="10" t="s">
+      <c r="Z11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z11" s="10" t="s">
+      <c r="AA11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA11" s="6" t="s">
+      <c r="AB11" t="s">
         <v>61</v>
       </c>
-      <c r="AD11" s="6" t="s">
+      <c r="AE11" t="s">
         <v>71</v>
       </c>
-      <c r="AE11" s="10" t="s">
+      <c r="AF11" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="1:34" ht="32">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" t="s">
         <v>110</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="L12" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="M12" t="s">
         <v>52</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="N12" t="s">
         <v>52</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="O12" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="Q12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="R12">
         <v>1</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="S12" t="s">
         <v>54</v>
       </c>
-      <c r="S12" s="6" t="s">
+      <c r="T12" t="s">
         <v>46</v>
       </c>
-      <c r="T12" s="6">
+      <c r="U12">
         <v>200</v>
       </c>
-      <c r="V12" s="6" t="s">
+      <c r="W12" t="s">
         <v>45</v>
       </c>
-      <c r="AB12" s="10" t="s">
+      <c r="AC12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AD12" s="6" t="s">
+      <c r="AE12" t="s">
         <v>52</v>
       </c>
-      <c r="AE12" s="10" t="s">
+      <c r="AF12" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B13" s="6" t="s">
+    <row r="13" spans="1:34" ht="32">
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" t="s">
         <v>110</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="L13" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="M13" t="s">
         <v>80</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="N13" t="s">
         <v>80</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="O13" t="s">
         <v>81</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="Q13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="R13">
         <v>2</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="S13" t="s">
         <v>54</v>
       </c>
-      <c r="S13" s="6" t="s">
+      <c r="T13" t="s">
         <v>46</v>
       </c>
-      <c r="T13" s="6">
+      <c r="U13">
         <v>200</v>
       </c>
-      <c r="V13" s="6" t="s">
+      <c r="W13" t="s">
         <v>45</v>
       </c>
-      <c r="AD13" s="6" t="s">
+      <c r="AE13" t="s">
         <v>80</v>
       </c>
-      <c r="AE13" s="10" t="s">
+      <c r="AF13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B14" s="6" t="s">
+    <row r="14" spans="1:34" ht="32">
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" t="s">
         <v>110</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="L14" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="M14" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" t="s">
         <v>43</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="O14" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="Q14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="R14">
         <v>3</v>
       </c>
-      <c r="R14" s="6" t="s">
+      <c r="S14" t="s">
         <v>45</v>
       </c>
-      <c r="S14" s="6" t="s">
+      <c r="T14" t="s">
         <v>46</v>
       </c>
-      <c r="T14" s="6">
+      <c r="U14">
         <v>200</v>
       </c>
-      <c r="AD14" s="6" t="s">
+      <c r="AE14" t="s">
         <v>43</v>
       </c>
-      <c r="AE14" s="10" t="s">
+      <c r="AF14" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:34" ht="32">
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
         <v>113</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" t="s">
         <v>76</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="N15" t="s">
         <v>76</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="O15" t="s">
         <v>78</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="Q15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="R15">
         <v>4</v>
       </c>
-      <c r="R15" s="6" t="s">
+      <c r="S15" t="s">
         <v>45</v>
       </c>
-      <c r="S15" s="6" t="s">
+      <c r="T15" t="s">
         <v>46</v>
       </c>
-      <c r="T15" s="6">
+      <c r="U15">
         <v>1</v>
       </c>
-      <c r="V15" s="6" t="s">
+      <c r="W15" t="s">
         <v>45</v>
       </c>
-      <c r="W15" s="6" t="s">
+      <c r="X15" t="s">
         <v>59</v>
       </c>
-      <c r="X15" s="11" t="s">
+      <c r="Y15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AB15" s="6" t="s">
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AC15" t="s">
         <v>45</v>
       </c>
-      <c r="AC15" s="6" t="s">
+      <c r="AD15" t="s">
         <v>84</v>
       </c>
-      <c r="AD15" s="6" t="s">
+      <c r="AE15" t="s">
         <v>76</v>
       </c>
-      <c r="AE15" s="10" t="s">
+      <c r="AF15" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="6" customFormat="1" ht="32">
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:34" ht="32">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="M16" t="s">
         <v>77</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="N16" t="s">
         <v>77</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="O16" t="s">
         <v>79</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="Q16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="R16">
         <v>5</v>
       </c>
-      <c r="R16" s="6" t="s">
+      <c r="S16" t="s">
         <v>45</v>
       </c>
-      <c r="S16" s="6" t="s">
+      <c r="T16" t="s">
         <v>46</v>
       </c>
-      <c r="T16" s="6">
+      <c r="U16">
         <v>1</v>
       </c>
-      <c r="W16" s="6" t="s">
+      <c r="X16" t="s">
         <v>59</v>
       </c>
-      <c r="X16" s="11" t="s">
+      <c r="Y16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y16" s="10" t="s">
+      <c r="Z16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" s="10" t="s">
+      <c r="AA16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA16" s="6" t="s">
+      <c r="AB16" t="s">
         <v>61</v>
       </c>
-      <c r="AD16" s="6" t="s">
+      <c r="AE16" t="s">
         <v>77</v>
       </c>
-      <c r="AE16" s="10" t="s">
+      <c r="AF16" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="2:32" ht="32">
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" t="s">
         <v>110</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="L17" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" t="s">
         <v>47</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="N17" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="O17" t="s">
         <v>56</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="Q17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="R17">
         <v>6</v>
       </c>
-      <c r="R17" s="6" t="s">
+      <c r="S17" t="s">
         <v>45</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="T17" t="s">
         <v>64</v>
       </c>
-      <c r="T17" s="6">
+      <c r="U17">
         <v>10</v>
       </c>
-      <c r="AD17" s="6" t="s">
+      <c r="AE17" t="s">
         <v>48</v>
       </c>
-      <c r="AE17" s="10" t="s">
+      <c r="AF17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="2:32" ht="32">
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="M18" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="N18" t="s">
         <v>50</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="O18" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="10" t="s">
+      <c r="Q18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="R18">
         <v>7</v>
       </c>
-      <c r="R18" s="6" t="s">
+      <c r="S18" t="s">
         <v>54</v>
       </c>
-      <c r="S18" s="6" t="s">
+      <c r="T18" t="s">
         <v>64</v>
       </c>
-      <c r="T18" s="6">
+      <c r="U18">
         <v>10</v>
       </c>
-      <c r="AD18" s="6" t="s">
+      <c r="AE18" t="s">
         <v>51</v>
       </c>
-      <c r="AE18" s="10" t="s">
+      <c r="AF18" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:31" s="6" customFormat="1" ht="48">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:32" ht="48">
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" t="s">
         <v>110</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="L19" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="M19" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="N19" t="s">
         <v>49</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="O19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="Q19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="R19">
         <v>8</v>
       </c>
-      <c r="R19" s="6" t="s">
+      <c r="S19" t="s">
         <v>54</v>
       </c>
-      <c r="S19" s="6" t="s">
+      <c r="T19" t="s">
         <v>46</v>
       </c>
-      <c r="T19" s="6">
+      <c r="U19">
         <v>1</v>
       </c>
-      <c r="W19" s="6" t="s">
+      <c r="X19" t="s">
         <v>59</v>
       </c>
-      <c r="X19" s="11" t="s">
+      <c r="Y19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y19" s="10" t="s">
+      <c r="Z19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z19" s="10" t="s">
+      <c r="AA19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA19" s="6" t="s">
+      <c r="AB19" t="s">
         <v>61</v>
       </c>
-      <c r="AD19" s="6" t="s">
+      <c r="AE19" t="s">
         <v>71</v>
       </c>
-      <c r="AE19" s="10" t="s">
+      <c r="AF19" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="2:32" ht="32">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="6" t="s">
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
         <v>115</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" t="s">
         <v>116</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20">
+        <v>360</v>
+      </c>
+      <c r="L20" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="M20" t="s">
         <v>43</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="N20" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="O20" t="s">
         <v>44</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="Q20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q20" s="6">
+      <c r="R20">
         <v>1</v>
       </c>
-      <c r="R20" s="6" t="s">
+      <c r="S20" t="s">
         <v>45</v>
       </c>
-      <c r="S20" s="6" t="s">
+      <c r="T20" t="s">
         <v>46</v>
       </c>
-      <c r="T20" s="6">
+      <c r="U20">
         <v>200</v>
       </c>
-      <c r="AB20" s="7" t="s">
+      <c r="AC20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AD20" s="6" t="s">
+      <c r="AE20" t="s">
         <v>43</v>
       </c>
-      <c r="AE20" s="10" t="s">
+      <c r="AF20" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="2:32" ht="32">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
         <v>115</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" t="s">
         <v>116</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K21">
+        <v>360</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="M21" t="s">
         <v>76</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="N21" t="s">
         <v>76</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="O21" t="s">
         <v>78</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="Q21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q21" s="6">
+      <c r="R21">
         <v>2</v>
       </c>
-      <c r="R21" s="6" t="s">
+      <c r="S21" t="s">
         <v>45</v>
       </c>
-      <c r="S21" s="6" t="s">
+      <c r="T21" t="s">
         <v>46</v>
       </c>
-      <c r="T21" s="6">
+      <c r="U21">
         <v>1</v>
       </c>
-      <c r="V21" s="6" t="s">
+      <c r="W21" t="s">
         <v>45</v>
       </c>
-      <c r="W21" s="6" t="s">
+      <c r="X21" t="s">
         <v>59</v>
       </c>
-      <c r="X21" s="11" t="s">
+      <c r="Y21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y21" s="10"/>
-      <c r="Z21" s="10"/>
-      <c r="AB21" s="6" t="s">
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AC21" t="s">
         <v>45</v>
       </c>
-      <c r="AC21" s="6" t="s">
+      <c r="AD21" t="s">
         <v>84</v>
       </c>
-      <c r="AD21" s="6" t="s">
+      <c r="AE21" t="s">
         <v>76</v>
       </c>
-      <c r="AE21" s="10" t="s">
+      <c r="AF21" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:32" ht="32">
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="6" t="s">
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
         <v>115</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" t="s">
         <v>116</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22">
+        <v>360</v>
+      </c>
+      <c r="L22" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="M22" t="s">
         <v>77</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="N22" t="s">
         <v>77</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="O22" t="s">
         <v>79</v>
       </c>
-      <c r="P22" s="10" t="s">
+      <c r="Q22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q22" s="6">
+      <c r="R22">
         <v>3</v>
       </c>
-      <c r="R22" s="6" t="s">
+      <c r="S22" t="s">
         <v>54</v>
       </c>
-      <c r="S22" s="6" t="s">
+      <c r="T22" t="s">
         <v>46</v>
       </c>
-      <c r="T22" s="6">
+      <c r="U22">
         <v>1</v>
       </c>
-      <c r="V22" s="6" t="s">
+      <c r="W22" t="s">
         <v>45</v>
       </c>
-      <c r="W22" s="6" t="s">
+      <c r="X22" t="s">
         <v>59</v>
       </c>
-      <c r="X22" s="11" t="s">
+      <c r="Y22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="10"/>
-      <c r="AB22" s="6" t="s">
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AC22" t="s">
         <v>45</v>
       </c>
-      <c r="AC22" s="6" t="s">
+      <c r="AD22" t="s">
         <v>84</v>
       </c>
-      <c r="AD22" s="6" t="s">
+      <c r="AE22" t="s">
         <v>77</v>
       </c>
-      <c r="AE22" s="10" t="s">
+      <c r="AF22" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="2:32" ht="32">
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="6" t="s">
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
         <v>115</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" t="s">
         <v>116</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23">
+        <v>360</v>
+      </c>
+      <c r="L23" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="M23" t="s">
         <v>94</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="N23" t="s">
         <v>94</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="Q23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="R23">
         <v>4</v>
       </c>
-      <c r="R23" s="6" t="s">
+      <c r="S23" t="s">
         <v>45</v>
       </c>
-      <c r="S23" s="6" t="s">
+      <c r="T23" t="s">
         <v>46</v>
       </c>
-      <c r="T23" s="6">
+      <c r="U23">
         <v>100</v>
       </c>
-      <c r="V23" s="6" t="s">
+      <c r="W23" t="s">
         <v>45</v>
       </c>
-      <c r="W23" s="6" t="s">
+      <c r="X23" t="s">
         <v>97</v>
       </c>
-      <c r="X23" s="7" t="s">
+      <c r="Y23" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AB23" s="6" t="s">
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AC23" t="s">
         <v>93</v>
       </c>
-      <c r="AC23" s="6" t="s">
+      <c r="AD23" t="s">
         <v>96</v>
       </c>
-      <c r="AD23" s="10" t="s">
+      <c r="AE23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AE23" s="10" t="s">
+      <c r="AF23" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="2:32" ht="32">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="6" t="s">
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" t="s">
         <v>115</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" t="s">
         <v>116</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24">
+        <v>360</v>
+      </c>
+      <c r="L24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="M24" t="s">
         <v>47</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="N24" t="s">
         <v>47</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="O24" t="s">
         <v>56</v>
       </c>
-      <c r="P24" s="10" t="s">
+      <c r="Q24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q24" s="6">
+      <c r="R24">
         <v>5</v>
       </c>
-      <c r="R24" s="6" t="s">
+      <c r="S24" t="s">
         <v>45</v>
       </c>
-      <c r="S24" s="6" t="s">
+      <c r="T24" t="s">
         <v>64</v>
       </c>
-      <c r="T24" s="6">
+      <c r="U24">
         <v>10</v>
       </c>
-      <c r="AD24" s="6" t="s">
+      <c r="AE24" t="s">
         <v>48</v>
       </c>
-      <c r="AE24" s="10" t="s">
+      <c r="AF24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:31" s="6" customFormat="1" ht="32">
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="2:32" ht="32">
+      <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="6" t="s">
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" t="s">
         <v>115</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" t="s">
         <v>116</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25">
+        <v>360</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="M25" t="s">
         <v>49</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="N25" t="s">
         <v>49</v>
       </c>
-      <c r="N25" s="11" t="s">
+      <c r="O25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="P25" s="10" t="s">
+      <c r="Q25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="R25">
         <v>6</v>
       </c>
-      <c r="R25" s="6" t="s">
+      <c r="S25" t="s">
         <v>54</v>
       </c>
-      <c r="S25" s="6" t="s">
+      <c r="T25" t="s">
         <v>46</v>
       </c>
-      <c r="T25" s="6">
+      <c r="U25">
         <v>1</v>
       </c>
-      <c r="V25" s="6" t="s">
+      <c r="W25" t="s">
         <v>45</v>
       </c>
-      <c r="W25" s="6" t="s">
+      <c r="X25" t="s">
         <v>59</v>
       </c>
-      <c r="X25" s="11" t="s">
+      <c r="Y25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Y25" s="10"/>
-      <c r="Z25" s="10"/>
-      <c r="AB25" s="6" t="s">
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AC25" t="s">
         <v>45</v>
       </c>
-      <c r="AC25" s="6" t="s">
+      <c r="AD25" t="s">
         <v>84</v>
       </c>
-      <c r="AD25" s="6" t="s">
+      <c r="AE25" t="s">
         <v>71</v>
       </c>
-      <c r="AE25" s="10" t="s">
+      <c r="AF25" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="2:31" s="6" customFormat="1">
-      <c r="E26" s="8"/>
-      <c r="K26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="AE26" s="10"/>
-    </row>
-    <row r="27" spans="2:31" s="6" customFormat="1">
-      <c r="E27" s="8"/>
-      <c r="K27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="AE27" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="W23" r:id="rId1" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C124301" xr:uid="{A9583DE8-5C3F-8146-8B2F-7E9240664096}"/>
+    <hyperlink ref="X23" r:id="rId1" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C124301" xr:uid="{A9583DE8-5C3F-8146-8B2F-7E9240664096}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added derivation columns (blank) - MH
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_MH.xlsx
+++ b/curation/draft/collection/collection_specialization_MH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C8A63-4769-D241-838E-B64ACF081A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EEBBC5-F4F5-4049-9253-8AFFC4659002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Collection_MH" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_MH!$A$1:$AH$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_MH!$A$1:$AJ$25</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="123">
   <si>
     <t>package_date</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>[NOT SUBMITTED];MHSTRF;MHSTRTPT;MHSTTPT</t>
+  </si>
+  <si>
+    <t>[NOT SUBMITTED];MHENRF;MHENRTPT;MHENTPT</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -789,12 +801,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH25"/>
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="112" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -813,16 +825,16 @@
     <col min="16" max="16" width="41.5" customWidth="1"/>
     <col min="17" max="17" width="23" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.1640625" customWidth="1"/>
-    <col min="24" max="24" width="18.6640625" customWidth="1"/>
-    <col min="25" max="25" width="24.5" customWidth="1"/>
-    <col min="29" max="29" width="15.33203125" customWidth="1"/>
-    <col min="30" max="30" width="25" customWidth="1"/>
-    <col min="31" max="31" width="29.33203125" customWidth="1"/>
-    <col min="32" max="32" width="23.83203125" style="1" customWidth="1"/>
+    <col min="23" max="25" width="13.1640625" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" customWidth="1"/>
+    <col min="27" max="27" width="24.5" customWidth="1"/>
+    <col min="31" max="31" width="15.33203125" customWidth="1"/>
+    <col min="32" max="32" width="25" customWidth="1"/>
+    <col min="33" max="33" width="29.33203125" customWidth="1"/>
+    <col min="34" max="34" width="23.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16">
+    <row r="1" spans="1:36" ht="16">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -893,40 +905,46 @@
         <v>21</v>
       </c>
       <c r="X1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="16">
+    <row r="2" spans="1:36" ht="16">
       <c r="B2" s="6" t="s">
         <v>55</v>
       </c>
@@ -969,26 +987,26 @@
       <c r="U2">
         <v>1</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="16">
+    <row r="3" spans="1:36" ht="16">
       <c r="B3" s="6" t="s">
         <v>55</v>
       </c>
@@ -1031,17 +1049,17 @@
       <c r="U3">
         <v>10</v>
       </c>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AE3" t="s">
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AG3" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="32">
+    <row r="4" spans="1:36" ht="32">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -1093,17 +1111,17 @@
       <c r="W4" t="s">
         <v>45</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>52</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="32">
+    <row r="5" spans="1:36" ht="32">
       <c r="B5" t="s">
         <v>41</v>
       </c>
@@ -1155,14 +1173,14 @@
       <c r="W5" t="s">
         <v>45</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>80</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AH5" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="32">
+    <row r="6" spans="1:36" ht="32">
       <c r="B6" s="6" t="s">
         <v>55</v>
       </c>
@@ -1208,14 +1226,14 @@
       <c r="U6">
         <v>2</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>69</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="32">
+    <row r="7" spans="1:36" ht="32">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -1264,14 +1282,14 @@
       <c r="U7">
         <v>200</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>43</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="32">
+    <row r="8" spans="1:36" ht="32">
       <c r="B8" t="s">
         <v>41</v>
       </c>
@@ -1320,14 +1338,14 @@
       <c r="U8">
         <v>10</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>48</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AH8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="32">
+    <row r="9" spans="1:36" ht="48">
       <c r="B9" t="s">
         <v>41</v>
       </c>
@@ -1374,29 +1392,29 @@
       <c r="U9">
         <v>1</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z9" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="8" t="s">
+      <c r="AA9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AD9" t="s">
         <v>61</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AG9" t="s">
         <v>74</v>
       </c>
-      <c r="AF9" s="1" t="s">
-        <v>74</v>
+      <c r="AH9" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="32">
+    <row r="10" spans="1:36" ht="32">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -1445,14 +1463,14 @@
       <c r="U10">
         <v>10</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" t="s">
         <v>51</v>
       </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AH10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="48">
+    <row r="11" spans="1:36" ht="48">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -1501,29 +1519,29 @@
       <c r="U11">
         <v>1</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>59</v>
       </c>
-      <c r="Y11" s="8" t="s">
+      <c r="AA11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AD11" t="s">
         <v>61</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AG11" t="s">
         <v>71</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AH11" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="32">
+    <row r="12" spans="1:36" ht="32">
       <c r="B12" t="s">
         <v>41</v>
       </c>
@@ -1575,17 +1593,17 @@
       <c r="W12" t="s">
         <v>45</v>
       </c>
-      <c r="AC12" s="1" t="s">
+      <c r="AE12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>52</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AH12" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="32">
+    <row r="13" spans="1:36" ht="32">
       <c r="B13" t="s">
         <v>41</v>
       </c>
@@ -1637,14 +1655,14 @@
       <c r="W13" t="s">
         <v>45</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>80</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AH13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="32">
+    <row r="14" spans="1:36" ht="32">
       <c r="B14" t="s">
         <v>41</v>
       </c>
@@ -1693,14 +1711,14 @@
       <c r="U14">
         <v>200</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>43</v>
       </c>
-      <c r="AF14" s="1" t="s">
+      <c r="AH14" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="32">
+    <row r="15" spans="1:36" ht="32">
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1752,28 +1770,28 @@
       <c r="W15" t="s">
         <v>45</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Z15" t="s">
         <v>59</v>
       </c>
-      <c r="Y15" s="8" t="s">
+      <c r="AA15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AC15" t="s">
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AE15" t="s">
         <v>45</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AF15" t="s">
         <v>84</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AG15" t="s">
         <v>76</v>
       </c>
-      <c r="AF15" s="1" t="s">
+      <c r="AH15" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="32">
+    <row r="16" spans="1:36" ht="32">
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -1822,29 +1840,29 @@
       <c r="U16">
         <v>1</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Z16" t="s">
         <v>59</v>
       </c>
-      <c r="Y16" s="8" t="s">
+      <c r="AA16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z16" s="1" t="s">
+      <c r="AB16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA16" s="1" t="s">
+      <c r="AC16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
         <v>61</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>77</v>
       </c>
-      <c r="AF16" s="1" t="s">
+      <c r="AH16" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="32">
+    <row r="17" spans="2:34" ht="32">
       <c r="B17" t="s">
         <v>41</v>
       </c>
@@ -1893,14 +1911,14 @@
       <c r="U17">
         <v>10</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AG17" t="s">
         <v>48</v>
       </c>
-      <c r="AF17" s="1" t="s">
+      <c r="AH17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:32" ht="32">
+    <row r="18" spans="2:34" ht="32">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -1949,14 +1967,14 @@
       <c r="U18">
         <v>10</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AG18" t="s">
         <v>51</v>
       </c>
-      <c r="AF18" s="1" t="s">
+      <c r="AH18" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:32" ht="48">
+    <row r="19" spans="2:34" ht="48">
       <c r="B19" t="s">
         <v>41</v>
       </c>
@@ -2005,29 +2023,29 @@
       <c r="U19">
         <v>1</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Z19" t="s">
         <v>59</v>
       </c>
-      <c r="Y19" s="8" t="s">
+      <c r="AA19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z19" s="1" t="s">
+      <c r="AB19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA19" s="1" t="s">
+      <c r="AC19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AD19" t="s">
         <v>61</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AG19" t="s">
         <v>71</v>
       </c>
-      <c r="AF19" s="1" t="s">
-        <v>71</v>
+      <c r="AH19" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="20" spans="2:32" ht="32">
+    <row r="20" spans="2:34" ht="32">
       <c r="B20" t="s">
         <v>41</v>
       </c>
@@ -2079,17 +2097,17 @@
       <c r="U20">
         <v>200</v>
       </c>
-      <c r="AC20" s="6" t="s">
+      <c r="AE20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AG20" t="s">
         <v>43</v>
       </c>
-      <c r="AF20" s="1" t="s">
+      <c r="AH20" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="2:32" ht="32">
+    <row r="21" spans="2:34" ht="32">
       <c r="B21" t="s">
         <v>41</v>
       </c>
@@ -2144,28 +2162,28 @@
       <c r="W21" t="s">
         <v>45</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Z21" t="s">
         <v>59</v>
       </c>
-      <c r="Y21" s="8" t="s">
+      <c r="AA21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AC21" t="s">
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AE21" t="s">
         <v>45</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AF21" t="s">
         <v>84</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AG21" t="s">
         <v>76</v>
       </c>
-      <c r="AF21" s="1" t="s">
+      <c r="AH21" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="2:32" ht="32">
+    <row r="22" spans="2:34" ht="32">
       <c r="B22" t="s">
         <v>41</v>
       </c>
@@ -2220,28 +2238,28 @@
       <c r="W22" t="s">
         <v>45</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Z22" t="s">
         <v>59</v>
       </c>
-      <c r="Y22" s="8" t="s">
+      <c r="AA22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AC22" t="s">
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AE22" t="s">
         <v>45</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AF22" t="s">
         <v>84</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AG22" t="s">
         <v>77</v>
       </c>
-      <c r="AF22" s="1" t="s">
+      <c r="AH22" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="2:32" ht="32">
+    <row r="23" spans="2:34" ht="32">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2293,28 +2311,28 @@
       <c r="W23" t="s">
         <v>45</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Z23" t="s">
         <v>97</v>
       </c>
-      <c r="Y23" s="6" t="s">
+      <c r="AA23" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AC23" t="s">
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AE23" t="s">
         <v>93</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AF23" t="s">
         <v>96</v>
       </c>
-      <c r="AE23" s="1" t="s">
+      <c r="AG23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AF23" s="1" t="s">
+      <c r="AH23" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="2:32" ht="32">
+    <row r="24" spans="2:34" ht="32">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -2366,14 +2384,14 @@
       <c r="U24">
         <v>10</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AG24" t="s">
         <v>48</v>
       </c>
-      <c r="AF24" s="1" t="s">
+      <c r="AH24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:32" ht="32">
+    <row r="25" spans="2:34" ht="32">
       <c r="B25" t="s">
         <v>41</v>
       </c>
@@ -2428,32 +2446,32 @@
       <c r="W25" t="s">
         <v>45</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Z25" t="s">
         <v>59</v>
       </c>
-      <c r="Y25" s="8" t="s">
+      <c r="AA25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AC25" t="s">
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AE25" t="s">
         <v>45</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AF25" t="s">
         <v>84</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AG25" t="s">
         <v>71</v>
       </c>
-      <c r="AF25" s="1" t="s">
+      <c r="AH25" s="1" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="X23" r:id="rId1" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C124301" xr:uid="{A9583DE8-5C3F-8146-8B2F-7E9240664096}"/>
+    <hyperlink ref="Z23" r:id="rId1" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C124301" xr:uid="{A9583DE8-5C3F-8146-8B2F-7E9240664096}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>